<commit_message>
googleTranslator api is imported
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
+++ b/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\Output2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4E656-3664-462E-B95A-5D4145E1D2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA7FB1F2-887D-49C6-9C70-404B63020C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="11064" windowHeight="5688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2697,11 +2697,13 @@
       <c r="D26" s="14"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
       <c r="H26" s="13"/>
       <c r="I26" s="17">
         <f>K26*G26</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>60</v>
@@ -2840,7 +2842,7 @@
       <c r="H32" s="47"/>
       <c r="I32" s="29">
         <f>SUM(I9:I31)</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="J32" s="18"/>
       <c r="K32" s="11"/>

</xml_diff>

<commit_message>
Extracted year & term successfully
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
+++ b/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\Output2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA7FB1F2-887D-49C6-9C70-404B63020C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4AA8B71-447E-40D5-93DB-1A481F77161D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="11064" windowHeight="5688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11844" yWindow="2832" windowWidth="11064" windowHeight="5688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Read write in excel almost done
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
+++ b/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\Output2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4AA8B71-447E-40D5-93DB-1A481F77161D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02A3E97B-8EC2-4033-94EB-04551852E09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11844" yWindow="2832" windowWidth="11064" windowHeight="5688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -228,15 +228,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>খুলনা প্রকৌশল ও প্রযু্ক্তি বিশ্ববিদ্যালয়</t>
   </si>
   <si>
     <t>পরীক্ষা সংক্রান্ত কাজের বিল ফর্ম</t>
-  </si>
-  <si>
-    <t>নিয়মিত পরীক্ষা ২০২২</t>
   </si>
   <si>
     <t>বর্ষ :</t>
@@ -497,19 +494,31 @@
     <t>অনুমোদনকারীঃ</t>
   </si>
   <si>
-    <t>নাম:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">পদবী: </t>
-  </si>
-  <si>
-    <t>বিভাগ :</t>
-  </si>
-  <si>
     <t>বিভাগ/শাখা:</t>
   </si>
   <si>
-    <t>কথায়:</t>
+    <t>নিয়মিত পরীক্ষা ২০২২</t>
+  </si>
+  <si>
+    <t>৪র্থ</t>
+  </si>
+  <si>
+    <t>১ম</t>
+  </si>
+  <si>
+    <t>সিএসই</t>
+  </si>
+  <si>
+    <t xml:space="preserve">নাম: Dr. A. R. M. Jalal Uddin Jamali </t>
+  </si>
+  <si>
+    <t>পদবী: অধ্যাপক</t>
+  </si>
+  <si>
+    <t>বিভাগ :গণিত</t>
+  </si>
+  <si>
+    <t>কথায়:দুই হাজার সাতশো টাকা মাত্র।</t>
   </si>
 </sst>
 </file>
@@ -2134,13 +2143,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="35" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" style="35" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" style="35" customWidth="1"/>
@@ -2184,14 +2193,14 @@
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1">
       <c r="A3" s="36" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="36" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
@@ -2199,31 +2208,37 @@
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
       <c r="A4" s="36" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1">
       <c r="A5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="2"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="36" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
@@ -2231,7 +2246,7 @@
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
       <c r="A6" s="41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -2257,43 +2272,43 @@
     </row>
     <row r="8" spans="1:11" ht="55.2">
       <c r="A8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1">
       <c r="A9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
@@ -2306,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="19">
         <v>3600</v>
@@ -2314,10 +2329,10 @@
     </row>
     <row r="10" spans="1:11" ht="39.75" customHeight="1">
       <c r="A10" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>20</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="20"/>
@@ -2330,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="19">
         <v>4500</v>
@@ -2339,7 +2354,7 @@
     <row r="11" spans="1:11" ht="21" customHeight="1">
       <c r="A11" s="42"/>
       <c r="B11" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
@@ -2352,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="19">
         <v>4500</v>
@@ -2360,10 +2375,10 @@
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1">
       <c r="A12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="14"/>
@@ -2376,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K12" s="19">
         <v>90</v>
@@ -2385,7 +2400,7 @@
     <row r="13" spans="1:11" ht="21" customHeight="1">
       <c r="A13" s="44"/>
       <c r="B13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="14"/>
@@ -2398,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K13" s="19">
         <v>50</v>
@@ -2407,7 +2422,7 @@
     <row r="14" spans="1:11" ht="21" customHeight="1">
       <c r="A14" s="45"/>
       <c r="B14" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -2420,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K14" s="19">
         <v>45</v>
@@ -2428,10 +2443,10 @@
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1">
       <c r="A15" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -2444,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="19">
         <v>600</v>
@@ -2453,10 +2468,10 @@
     <row r="16" spans="1:11" ht="21" customHeight="1">
       <c r="A16" s="44"/>
       <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="13"/>
@@ -2470,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="19">
         <v>300</v>
@@ -2479,7 +2494,7 @@
     <row r="17" spans="1:11" ht="21" customHeight="1">
       <c r="A17" s="44"/>
       <c r="B17" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
@@ -2492,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K17" s="19">
         <v>300</v>
@@ -2501,7 +2516,7 @@
     <row r="18" spans="1:11" ht="21" customHeight="1">
       <c r="A18" s="45"/>
       <c r="B18" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
@@ -2516,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K18" s="19">
         <v>150</v>
@@ -2524,10 +2539,10 @@
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1">
       <c r="A19" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -2540,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K19" s="19">
         <v>2400</v>
@@ -2549,10 +2564,10 @@
     <row r="20" spans="1:11" ht="26.25" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="20"/>
@@ -2564,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20" s="19">
         <v>100</v>
@@ -2573,7 +2588,7 @@
     <row r="21" spans="1:11" ht="26.25" customHeight="1">
       <c r="A21" s="42"/>
       <c r="B21" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
@@ -2586,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K21" s="19">
         <v>225</v>
@@ -2595,7 +2610,7 @@
     <row r="22" spans="1:11" ht="21" customHeight="1">
       <c r="A22" s="42"/>
       <c r="B22" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -2608,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K22" s="19">
         <v>4500</v>
@@ -2616,10 +2631,10 @@
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1">
       <c r="A23" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
@@ -2632,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K23" s="19">
         <v>45</v>
@@ -2641,7 +2656,7 @@
     <row r="24" spans="1:11" ht="23.25" customHeight="1">
       <c r="A24" s="42"/>
       <c r="B24" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="14"/>
@@ -2654,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" s="19">
         <v>20</v>
@@ -2662,10 +2677,10 @@
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1">
       <c r="A25" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="14"/>
@@ -2678,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K25" s="19">
         <v>10</v>
@@ -2686,13 +2701,13 @@
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1">
       <c r="A26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="C26" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="13"/>
@@ -2706,7 +2721,7 @@
         <v>2700</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K26" s="19">
         <v>2700</v>
@@ -2714,13 +2729,13 @@
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1">
       <c r="A27" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>62</v>
-      </c>
       <c r="C27" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="20"/>
@@ -2732,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K27" s="19">
         <v>1500</v>
@@ -2740,13 +2755,13 @@
     </row>
     <row r="28" spans="1:11" ht="27.75" customHeight="1">
       <c r="A28" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="C28" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="13"/>
@@ -2758,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K28" s="19">
         <v>900</v>
@@ -2767,7 +2782,7 @@
     <row r="29" spans="1:11" ht="21" customHeight="1">
       <c r="A29" s="42"/>
       <c r="B29" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
@@ -2780,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K29" s="19">
         <v>225</v>
@@ -2788,10 +2803,10 @@
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1">
       <c r="A30" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>70</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -2805,10 +2820,10 @@
     </row>
     <row r="31" spans="1:11" ht="18.75" customHeight="1">
       <c r="A31" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -2821,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K31" s="26">
         <v>3600</v>
@@ -2829,7 +2844,7 @@
     </row>
     <row r="32" spans="1:11" ht="20.25" customHeight="1">
       <c r="A32" s="46" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B32" s="46"/>
       <c r="C32" s="46"/>
@@ -2837,7 +2852,7 @@
       <c r="E32" s="46"/>
       <c r="F32" s="27"/>
       <c r="G32" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H32" s="47"/>
       <c r="I32" s="29">
@@ -2873,7 +2888,7 @@
     </row>
     <row r="35" spans="1:10" ht="16.5" customHeight="1">
       <c r="A35" s="46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="46"/>
       <c r="C35" s="27"/>
@@ -2885,16 +2900,16 @@
       <c r="I35" s="27"/>
       <c r="J35" s="31"/>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1">
+    <row r="36" spans="1:10" ht="68.400000000000006" customHeight="1">
       <c r="A36" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
       <c r="F36" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G36" s="40"/>
       <c r="H36" s="40"/>
@@ -2903,14 +2918,14 @@
     </row>
     <row r="37" spans="1:10" ht="38.25" customHeight="1">
       <c r="A37" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
@@ -2919,7 +2934,7 @@
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
       <c r="A38" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="47"/>
       <c r="C38" s="47"/>
@@ -2945,7 +2960,7 @@
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
       <c r="A40" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="47"/>
       <c r="C40" s="47"/>
@@ -2959,7 +2974,7 @@
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
@@ -2973,7 +2988,7 @@
     </row>
     <row r="42" spans="1:10" ht="23.25" customHeight="1">
       <c r="A42" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="50"/>
       <c r="C42" s="27"/>
@@ -2982,7 +2997,7 @@
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
       <c r="H42" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I42" s="48"/>
       <c r="J42" s="31"/>
@@ -3002,19 +3017,19 @@
     <row r="44" spans="1:10" ht="30" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="31"/>

</xml_diff>

<commit_message>
Implemented Label wise bill generate(Individual)
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
+++ b/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\Output2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02A758E1-3B48-40E4-9C26-CDDC3FABE5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F711484E-E9EA-4C40-A06B-27A1DD5200D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2592" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9828" yWindow="6132" windowWidth="12408" windowHeight="5472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,21 +494,9 @@
     <t>অনুমোদনকারীঃ</t>
   </si>
   <si>
-    <t xml:space="preserve">পদবী: </t>
-  </si>
-  <si>
-    <t>বিভাগ :</t>
-  </si>
-  <si>
     <t>বিভাগ/শাখা:</t>
   </si>
   <si>
-    <t>কথায়:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">নাম: </t>
-  </si>
-  <si>
     <t>নিয়মিত পরীক্ষা ২০২২</t>
   </si>
   <si>
@@ -519,6 +507,18 @@
   </si>
   <si>
     <t>সিএসই</t>
+  </si>
+  <si>
+    <t xml:space="preserve">নাম: Dr. A. R. M. Jalal Uddin Jamali </t>
+  </si>
+  <si>
+    <t>পদবী: অধ্যাপক</t>
+  </si>
+  <si>
+    <t>বিভাগ :গণিত</t>
+  </si>
+  <si>
+    <t>কথায়:দুই হাজার সাতশো টাকা মাত্র।</t>
   </si>
 </sst>
 </file>
@@ -827,49 +827,49 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2144,7 +2144,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>
@@ -2164,98 +2164,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1">
-      <c r="A3" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
+      <c r="A3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
+      <c r="F3" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
+      <c r="A4" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="F5" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="6" customHeight="1">
@@ -2328,7 +2328,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="39.75" customHeight="1">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1">
-      <c r="A11" s="43"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1">
-      <c r="A13" s="45"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2420,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1">
-      <c r="A14" s="46"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="13" t="s">
         <v>28</v>
       </c>
@@ -2442,7 +2442,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -2466,7 +2466,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1">
-      <c r="A16" s="45"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="13" t="s">
         <v>33</v>
       </c>
@@ -2492,7 +2492,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1">
-      <c r="A17" s="45"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1">
-      <c r="A18" s="46"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A20" s="43"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
@@ -2586,7 +2586,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A21" s="43"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="13" t="s">
         <v>45</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1">
-      <c r="A22" s="43"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="13" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2630,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A24" s="43"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="13" t="s">
         <v>52</v>
       </c>
@@ -2712,11 +2712,13 @@
       <c r="D26" s="14"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
       <c r="H26" s="13"/>
       <c r="I26" s="17">
         <f>K26*G26</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>59</v>
@@ -2752,7 +2754,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="13" t="s">
@@ -2778,7 +2780,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1">
-      <c r="A29" s="43"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="13" t="s">
         <v>66</v>
       </c>
@@ -2841,21 +2843,21 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A32" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
+      <c r="A32" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="39"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="29">
         <f>SUM(I9:I31)</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="J32" s="18"/>
       <c r="K32" s="11"/>
@@ -2876,8 +2878,8 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="27"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
@@ -2885,13 +2887,13 @@
       <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="47"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="27"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
@@ -2899,49 +2901,49 @@
       <c r="J35" s="31"/>
     </row>
     <row r="36" spans="1:10" ht="68.400000000000006" customHeight="1">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
-      <c r="F36" s="41" t="s">
+      <c r="F36" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
       <c r="J36" s="31"/>
     </row>
     <row r="37" spans="1:10" ht="38.25" customHeight="1">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
       <c r="J37" s="31"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
       <c r="J38" s="31"/>
     </row>
     <row r="39" spans="1:10" ht="13.5" customHeight="1">
@@ -2957,17 +2959,17 @@
       <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
       <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
@@ -2985,19 +2987,19 @@
       <c r="J41" s="31"/>
     </row>
     <row r="42" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
-      <c r="H42" s="38" t="s">
+      <c r="H42" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="38"/>
+      <c r="I42" s="48"/>
       <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" ht="13.8">
@@ -3214,12 +3216,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:I42"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="F36:I36"/>
     <mergeCell ref="A6:I6"/>
@@ -3233,12 +3235,12 @@
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="D34:E35"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="The date of this cell can't be changed or deleted." sqref="K45:K65536" xr:uid="{18A23E8D-DD15-4DD7-A5BE-6BF6836D2F72}">

</xml_diff>

<commit_message>
Show list of the created file
</commit_message>
<xml_diff>
--- a/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
+++ b/PDF to EXCEL/Project/Output2/DrARMJalalUddinJamali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\3rd Year\KUET 6th Sem\Laboratory\CSE 3200 System Development Project\PDF to EXCEL\Project\Output2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F711484E-E9EA-4C40-A06B-27A1DD5200D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1512A797-781C-4B43-8A33-943D83800432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9828" yWindow="6132" windowWidth="12408" windowHeight="5472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9300" yWindow="3060" windowWidth="12408" windowHeight="8256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -827,6 +827,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -834,42 +870,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2164,54 +2164,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
@@ -2237,25 +2237,25 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="6" customHeight="1">
@@ -2328,7 +2328,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="39.75" customHeight="1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2398,7 +2398,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1">
-      <c r="A13" s="44"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="13" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2420,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13" t="s">
         <v>28</v>
       </c>
@@ -2442,7 +2442,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -2466,7 +2466,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1">
-      <c r="A16" s="44"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="13" t="s">
         <v>33</v>
       </c>
@@ -2492,7 +2492,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1">
-      <c r="A17" s="44"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="43" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
@@ -2586,7 +2586,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="13" t="s">
         <v>45</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1">
-      <c r="A22" s="42"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="13" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2630,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="43" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A24" s="42"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="13" t="s">
         <v>52</v>
       </c>
@@ -2754,7 +2754,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="43" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="13" t="s">
@@ -2780,7 +2780,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1">
-      <c r="A29" s="42"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="13" t="s">
         <v>66</v>
       </c>
@@ -2843,18 +2843,18 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="47" t="s">
+      <c r="G32" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="47"/>
+      <c r="H32" s="39"/>
       <c r="I32" s="29">
         <f>SUM(I9:I31)</f>
         <v>2700</v>
@@ -2878,8 +2878,8 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="27"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
@@ -2887,13 +2887,13 @@
       <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="27"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
@@ -2901,49 +2901,49 @@
       <c r="J35" s="31"/>
     </row>
     <row r="36" spans="1:10" ht="68.400000000000006" customHeight="1">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
-      <c r="F36" s="40" t="s">
+      <c r="F36" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
       <c r="J36" s="31"/>
     </row>
     <row r="37" spans="1:10" ht="38.25" customHeight="1">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
       <c r="J37" s="31"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
       <c r="J38" s="31"/>
     </row>
     <row r="39" spans="1:10" ht="13.5" customHeight="1">
@@ -2959,17 +2959,17 @@
       <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
       <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
@@ -2987,19 +2987,19 @@
       <c r="J41" s="31"/>
     </row>
     <row r="42" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="50"/>
+      <c r="B42" s="40"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="48"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" ht="13.8">
@@ -3216,12 +3216,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="F36:I36"/>
     <mergeCell ref="A6:I6"/>
@@ -3235,12 +3235,12 @@
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="D34:E35"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:I42"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="The date of this cell can't be changed or deleted." sqref="K45:K65536" xr:uid="{18A23E8D-DD15-4DD7-A5BE-6BF6836D2F72}">

</xml_diff>